<commit_message>
bugfix + change object + disclaimer
</commit_message>
<xml_diff>
--- a/StepByStepToAnEasyJog/Table/Run.xlsx
+++ b/StepByStepToAnEasyJog/Table/Run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Progects in work\StepByStepToAnEasyJog\StepByStepToAnEasyJog\Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426E86BA-29AE-4485-8EB0-8B202D2A0280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C29927-4DE5-49EB-A03C-098C3FD1D773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="756" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="756" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Тренировочные фазы" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2394" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2396" uniqueCount="893">
   <si>
     <t>Фаза 1</t>
   </si>
@@ -2406,9 +2406,6 @@
     <t>В остальные дни можно проводить 60-минутные пробежки в темпе [L]</t>
   </si>
   <si>
-    <t>· 5–6 × (2 × (200 м за [Pov200] + 200 м бега трусцой) + (400 м за [Pov400] + 400 м бега трусцой))</t>
-  </si>
-  <si>
     <t>5–6 × (1600 м в темпе [P] + 1 мин отдыха)</t>
   </si>
   <si>
@@ -2716,6 +2713,9 @@
   </si>
   <si>
     <t>За 1 день до забега</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5–6 × </t>
   </si>
 </sst>
 </file>
@@ -43906,7 +43906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9177D02D-B379-427D-ABFA-2DB8BB488DC3}">
   <dimension ref="A1:B525"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+    <sheetView topLeftCell="A232" workbookViewId="0">
       <selection activeCell="B518" sqref="B518"/>
     </sheetView>
   </sheetViews>
@@ -49715,10 +49715,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9593F19-7502-4EED-B12C-F3DAD2133264}">
-  <dimension ref="A1:B461"/>
+  <dimension ref="A1:B464"/>
   <sheetViews>
-    <sheetView topLeftCell="A410" workbookViewId="0">
-      <selection activeCell="B455" sqref="B455"/>
+    <sheetView topLeftCell="A344" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -50279,209 +50279,209 @@
       </c>
       <c r="B104" s="5"/>
     </row>
-    <row r="105" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="8" t="s">
+        <v>892</v>
+      </c>
+      <c r="B105" s="5"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="B106" s="5"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="8" t="s">
+        <v>748</v>
+      </c>
+      <c r="B107" s="5"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="8"/>
+      <c r="B108" s="5"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="B109" s="5"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="8" t="s">
         <v>789</v>
       </c>
-      <c r="B105" s="5"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="8"/>
-      <c r="B106" s="5"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="9" t="s">
-        <v>654</v>
-      </c>
-      <c r="B107" s="5"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="B108" s="5"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="8"/>
-      <c r="B109" s="5"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="9" t="s">
+      <c r="B110" s="5"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="8"/>
+      <c r="B111" s="5"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="B110" s="5"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="8" t="s">
+      <c r="B112" s="5"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="8" t="s">
         <v>761</v>
-      </c>
-      <c r="B111" s="5"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="10" t="s">
-        <v>791</v>
-      </c>
-      <c r="B112" s="5"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="10" t="s">
-        <v>792</v>
       </c>
       <c r="B113" s="5"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="B114" s="5"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
+        <v>791</v>
+      </c>
+      <c r="B115" s="5"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="10" t="s">
+        <v>792</v>
+      </c>
+      <c r="B116" s="5"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="10" t="s">
+        <v>793</v>
+      </c>
+      <c r="B117" s="5"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="8"/>
+      <c r="B118" s="5"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="B119" s="5"/>
+    </row>
+    <row r="120" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A120" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="B120" s="5"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="8"/>
+      <c r="B121" s="5"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="B122" s="5"/>
+    </row>
+    <row r="123" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A123" s="8" t="s">
+        <v>695</v>
+      </c>
+      <c r="B123" s="5"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="8"/>
+      <c r="B124" s="5"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="8"/>
+      <c r="B125" s="5"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="B126" s="5"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="B127" s="5"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="8" t="s">
         <v>794</v>
       </c>
-      <c r="B115" s="5"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="8"/>
-      <c r="B116" s="5"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="9" t="s">
-        <v>656</v>
-      </c>
-      <c r="B117" s="5"/>
-    </row>
-    <row r="118" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A118" s="8" t="s">
+      <c r="B128" s="5"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="8"/>
+      <c r="B129" s="5"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="B130" s="5"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="8" t="s">
+        <v>795</v>
+      </c>
+      <c r="B131" s="5"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="8"/>
+      <c r="B132" s="5"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="9" t="s">
+        <v>655</v>
+      </c>
+      <c r="B133" s="5"/>
+    </row>
+    <row r="134" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A134" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="B118" s="5"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="8"/>
-      <c r="B119" s="5"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="9" t="s">
+      <c r="B134" s="5"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="8"/>
+      <c r="B135" s="5"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="9" t="s">
         <v>680</v>
       </c>
-      <c r="B120" s="5"/>
-    </row>
-    <row r="121" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A121" s="8" t="s">
+      <c r="B136" s="5"/>
+    </row>
+    <row r="137" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A137" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B121" s="5"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="8"/>
-      <c r="B122" s="5"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="8"/>
-      <c r="B123" s="5"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="7" t="s">
-        <v>657</v>
-      </c>
-      <c r="B124" s="5"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="9" t="s">
+      <c r="B137" s="5"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="8"/>
+      <c r="B138" s="5"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="8"/>
+      <c r="B139" s="5"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="B140" s="5"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="9" t="s">
         <v>653</v>
-      </c>
-      <c r="B125" s="5"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="8" t="s">
-        <v>795</v>
-      </c>
-      <c r="B126" s="5"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="8"/>
-      <c r="B127" s="5"/>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="9" t="s">
-        <v>654</v>
-      </c>
-      <c r="B128" s="5"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="8" t="s">
-        <v>796</v>
-      </c>
-      <c r="B129" s="5"/>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="8"/>
-      <c r="B130" s="5"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="9" t="s">
-        <v>655</v>
-      </c>
-      <c r="B131" s="5"/>
-    </row>
-    <row r="132" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A132" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="B132" s="5"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="8"/>
-      <c r="B133" s="5"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="9" t="s">
-        <v>680</v>
-      </c>
-      <c r="B134" s="5"/>
-    </row>
-    <row r="135" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A135" s="8" t="s">
-        <v>695</v>
-      </c>
-      <c r="B135" s="5"/>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="8"/>
-      <c r="B136" s="5"/>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="8"/>
-      <c r="B137" s="5"/>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="7" t="s">
-        <v>658</v>
-      </c>
-      <c r="B138" s="5"/>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="B139" s="5"/>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="8" t="s">
-        <v>712</v>
-      </c>
-      <c r="B140" s="5"/>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="8" t="s">
-        <v>763</v>
       </c>
       <c r="B141" s="5"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="8" t="s">
-        <v>723</v>
+        <v>712</v>
       </c>
       <c r="B142" s="5"/>
     </row>
@@ -50493,871 +50493,871 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="8" t="s">
+        <v>723</v>
+      </c>
+      <c r="B144" s="5"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="8" t="s">
+        <v>763</v>
+      </c>
+      <c r="B145" s="5"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="8" t="s">
         <v>712</v>
       </c>
-      <c r="B144" s="5"/>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="8"/>
-      <c r="B145" s="5"/>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="9" t="s">
+      <c r="B146" s="5"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="8"/>
+      <c r="B147" s="5"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="B146" s="5"/>
-    </row>
-    <row r="147" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A147" s="8" t="s">
+      <c r="B148" s="5"/>
+    </row>
+    <row r="149" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A149" s="8" t="s">
+        <v>796</v>
+      </c>
+      <c r="B149" s="5"/>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="8"/>
+      <c r="B150" s="5"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="9" t="s">
+        <v>655</v>
+      </c>
+      <c r="B151" s="5"/>
+    </row>
+    <row r="152" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A152" s="8" t="s">
         <v>797</v>
       </c>
-      <c r="B147" s="5"/>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="8"/>
-      <c r="B148" s="5"/>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="9" t="s">
-        <v>655</v>
-      </c>
-      <c r="B149" s="5"/>
-    </row>
-    <row r="150" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A150" s="8" t="s">
+      <c r="B152" s="5"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="8"/>
+      <c r="B153" s="5"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="B154" s="5"/>
+    </row>
+    <row r="155" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A155" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="B155" s="5"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="8"/>
+      <c r="B156" s="5"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="B157" s="5"/>
+    </row>
+    <row r="158" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A158" s="8" t="s">
+        <v>695</v>
+      </c>
+      <c r="B158" s="5"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="8"/>
+      <c r="B159" s="5"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="8"/>
+      <c r="B160" s="5"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="B161" s="5"/>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="B162" s="5"/>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="8" t="s">
         <v>798</v>
-      </c>
-      <c r="B150" s="5"/>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="8"/>
-      <c r="B151" s="5"/>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="9" t="s">
-        <v>656</v>
-      </c>
-      <c r="B152" s="5"/>
-    </row>
-    <row r="153" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A153" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="B153" s="5"/>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="8"/>
-      <c r="B154" s="5"/>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="9" t="s">
-        <v>680</v>
-      </c>
-      <c r="B155" s="5"/>
-    </row>
-    <row r="156" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A156" s="8" t="s">
-        <v>695</v>
-      </c>
-      <c r="B156" s="5"/>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="8"/>
-      <c r="B157" s="5"/>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="8"/>
-      <c r="B158" s="5"/>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="7" t="s">
-        <v>659</v>
-      </c>
-      <c r="B159" s="5"/>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="B160" s="5"/>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" s="8" t="s">
-        <v>799</v>
-      </c>
-      <c r="B161" s="5"/>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" s="10" t="s">
-        <v>725</v>
-      </c>
-      <c r="B162" s="5"/>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" s="10" t="s">
-        <v>800</v>
       </c>
       <c r="B163" s="5"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="10" t="s">
-        <v>801</v>
+        <v>725</v>
       </c>
       <c r="B164" s="5"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" s="8"/>
+      <c r="A165" s="10" t="s">
+        <v>799</v>
+      </c>
       <c r="B165" s="5"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" s="9" t="s">
+      <c r="A166" s="10" t="s">
+        <v>800</v>
+      </c>
+      <c r="B166" s="5"/>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="8"/>
+      <c r="B167" s="5"/>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="B166" s="5"/>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" s="8" t="s">
-        <v>796</v>
-      </c>
-      <c r="B167" s="5"/>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" s="8"/>
       <c r="B168" s="5"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" s="9" t="s">
+      <c r="A169" s="8" t="s">
+        <v>795</v>
+      </c>
+      <c r="B169" s="5"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="8"/>
+      <c r="B170" s="5"/>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="B169" s="5"/>
-    </row>
-    <row r="170" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A170" s="8" t="s">
+      <c r="B171" s="5"/>
+    </row>
+    <row r="172" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A172" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="B170" s="5"/>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" s="8"/>
-      <c r="B171" s="5"/>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" s="9" t="s">
+      <c r="B172" s="5"/>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="8"/>
+      <c r="B173" s="5"/>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="9" t="s">
         <v>680</v>
       </c>
-      <c r="B172" s="5"/>
-    </row>
-    <row r="173" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A173" s="8" t="s">
+      <c r="B174" s="5"/>
+    </row>
+    <row r="175" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A175" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B173" s="5"/>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" s="8"/>
-      <c r="B174" s="5"/>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" s="8"/>
       <c r="B175" s="5"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" s="7" t="s">
+      <c r="A176" s="8"/>
+      <c r="B176" s="5"/>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="8"/>
+      <c r="B177" s="5"/>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="7" t="s">
         <v>660</v>
       </c>
-      <c r="B176" s="5"/>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" s="9" t="s">
+      <c r="B178" s="5"/>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="B177" s="5"/>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" s="8" t="s">
-        <v>795</v>
-      </c>
-      <c r="B178" s="5"/>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" s="8"/>
       <c r="B179" s="5"/>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="9" t="s">
+      <c r="A180" s="8" t="s">
+        <v>794</v>
+      </c>
+      <c r="B180" s="5"/>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="8"/>
+      <c r="B181" s="5"/>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="9" t="s">
         <v>654</v>
-      </c>
-      <c r="B180" s="5"/>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" s="8" t="s">
-        <v>802</v>
-      </c>
-      <c r="B181" s="5"/>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" s="8" t="s">
-        <v>803</v>
       </c>
       <c r="B182" s="5"/>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="8" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="B183" s="5"/>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="8" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="B184" s="5"/>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="8" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B185" s="5"/>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A186" s="8"/>
+      <c r="A186" s="8" t="s">
+        <v>804</v>
+      </c>
       <c r="B186" s="5"/>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" s="9" t="s">
+      <c r="A187" s="8" t="s">
+        <v>805</v>
+      </c>
+      <c r="B187" s="5"/>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="8"/>
+      <c r="B188" s="5"/>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="B187" s="5"/>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" s="8" t="s">
+      <c r="B189" s="5"/>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="8" t="s">
         <v>761</v>
-      </c>
-      <c r="B188" s="5"/>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A189" s="10" t="s">
-        <v>791</v>
-      </c>
-      <c r="B189" s="5"/>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" s="10" t="s">
-        <v>792</v>
       </c>
       <c r="B190" s="5"/>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="10" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="B191" s="5"/>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="10" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="B192" s="5"/>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" s="8"/>
+      <c r="A193" s="10" t="s">
+        <v>792</v>
+      </c>
       <c r="B193" s="5"/>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A194" s="9" t="s">
+      <c r="A194" s="10" t="s">
+        <v>793</v>
+      </c>
+      <c r="B194" s="5"/>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="8"/>
+      <c r="B195" s="5"/>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="B194" s="5"/>
-    </row>
-    <row r="195" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A195" s="8" t="s">
+      <c r="B196" s="5"/>
+    </row>
+    <row r="197" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A197" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="B195" s="5"/>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A196" s="8"/>
-      <c r="B196" s="5"/>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" s="9" t="s">
+      <c r="B197" s="5"/>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="8"/>
+      <c r="B198" s="5"/>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="9" t="s">
         <v>680</v>
       </c>
-      <c r="B197" s="5"/>
-    </row>
-    <row r="198" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A198" s="8" t="s">
+      <c r="B199" s="5"/>
+    </row>
+    <row r="200" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A200" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B198" s="5"/>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A199" s="8"/>
-      <c r="B199" s="5"/>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A200" s="8"/>
       <c r="B200" s="5"/>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A201" s="7" t="s">
+      <c r="A201" s="8"/>
+      <c r="B201" s="5"/>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="8"/>
+      <c r="B202" s="5"/>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="7" t="s">
         <v>661</v>
       </c>
-      <c r="B201" s="5"/>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A202" s="9" t="s">
+      <c r="B203" s="5"/>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="B202" s="5"/>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A203" s="8" t="s">
-        <v>799</v>
-      </c>
-      <c r="B203" s="5"/>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A204" s="10" t="s">
-        <v>725</v>
-      </c>
       <c r="B204" s="5"/>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A205" s="10" t="s">
-        <v>800</v>
+      <c r="A205" s="8" t="s">
+        <v>798</v>
       </c>
       <c r="B205" s="5"/>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="10" t="s">
-        <v>801</v>
+        <v>725</v>
       </c>
       <c r="B206" s="5"/>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A207" s="8"/>
+      <c r="A207" s="10" t="s">
+        <v>799</v>
+      </c>
       <c r="B207" s="5"/>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A208" s="9" t="s">
+      <c r="A208" s="10" t="s">
+        <v>800</v>
+      </c>
+      <c r="B208" s="5"/>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" s="8"/>
+      <c r="B209" s="5"/>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" s="9" t="s">
         <v>654</v>
-      </c>
-      <c r="B208" s="5"/>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A209" s="8" t="s">
-        <v>807</v>
-      </c>
-      <c r="B209" s="5"/>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A210" s="8" t="s">
-        <v>808</v>
       </c>
       <c r="B210" s="5"/>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="8" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B211" s="5"/>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="8" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="B212" s="5"/>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="8" t="s">
-        <v>802</v>
+        <v>808</v>
       </c>
       <c r="B213" s="5"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="8" t="s">
-        <v>803</v>
+        <v>809</v>
       </c>
       <c r="B214" s="5"/>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="8" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="B215" s="5"/>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="8" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="B216" s="5"/>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="8" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B217" s="5"/>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A218" s="8"/>
+      <c r="A218" s="8" t="s">
+        <v>804</v>
+      </c>
       <c r="B218" s="5"/>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A219" s="9" t="s">
+      <c r="A219" s="8" t="s">
+        <v>805</v>
+      </c>
+      <c r="B219" s="5"/>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="8"/>
+      <c r="B220" s="5"/>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="B219" s="5"/>
-    </row>
-    <row r="220" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A220" s="8" t="s">
+      <c r="B221" s="5"/>
+    </row>
+    <row r="222" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A222" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="B220" s="5"/>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A221" s="8"/>
-      <c r="B221" s="5"/>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A222" s="9" t="s">
+      <c r="B222" s="5"/>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="8"/>
+      <c r="B223" s="5"/>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="9" t="s">
         <v>680</v>
       </c>
-      <c r="B222" s="5"/>
-    </row>
-    <row r="223" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A223" s="8" t="s">
+      <c r="B224" s="5"/>
+    </row>
+    <row r="225" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A225" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B223" s="5"/>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A224" s="8"/>
-      <c r="B224" s="5"/>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A225" s="8"/>
       <c r="B225" s="5"/>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A226" s="7" t="s">
+      <c r="A226" s="8"/>
+      <c r="B226" s="5"/>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="8"/>
+      <c r="B227" s="5"/>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="7" t="s">
         <v>662</v>
       </c>
-      <c r="B226" s="5"/>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A227" s="9" t="s">
+      <c r="B228" s="5"/>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="B227" s="5"/>
-    </row>
-    <row r="228" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A228" s="8" t="s">
+      <c r="B229" s="5"/>
+    </row>
+    <row r="230" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A230" s="8" t="s">
+        <v>810</v>
+      </c>
+      <c r="B230" s="5"/>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="8"/>
+      <c r="B231" s="5"/>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="B232" s="5"/>
+    </row>
+    <row r="233" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A233" s="8" t="s">
         <v>811</v>
       </c>
-      <c r="B228" s="5"/>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A229" s="8"/>
-      <c r="B229" s="5"/>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A230" s="9" t="s">
-        <v>654</v>
-      </c>
-      <c r="B230" s="5"/>
-    </row>
-    <row r="231" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A231" s="8" t="s">
-        <v>812</v>
-      </c>
-      <c r="B231" s="5"/>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A232" s="8"/>
-      <c r="B232" s="5"/>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A233" s="9" t="s">
+      <c r="B233" s="5"/>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" s="8"/>
+      <c r="B234" s="5"/>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="B233" s="5"/>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A234" s="8" t="s">
+      <c r="B235" s="5"/>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" s="8" t="s">
         <v>761</v>
-      </c>
-      <c r="B234" s="5"/>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A235" s="10" t="s">
-        <v>791</v>
-      </c>
-      <c r="B235" s="5"/>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A236" s="10" t="s">
-        <v>792</v>
       </c>
       <c r="B236" s="5"/>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="10" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="B237" s="5"/>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" s="10" t="s">
+        <v>791</v>
+      </c>
+      <c r="B238" s="5"/>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" s="10" t="s">
+        <v>792</v>
+      </c>
+      <c r="B239" s="5"/>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" s="10" t="s">
+        <v>793</v>
+      </c>
+      <c r="B240" s="5"/>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" s="8"/>
+      <c r="B241" s="5"/>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="B242" s="5"/>
+    </row>
+    <row r="243" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A243" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="B243" s="5"/>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" s="8"/>
+      <c r="B244" s="5"/>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="B245" s="5"/>
+    </row>
+    <row r="246" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A246" s="8" t="s">
+        <v>695</v>
+      </c>
+      <c r="B246" s="5"/>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" s="8"/>
+      <c r="B247" s="5"/>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" s="8"/>
+      <c r="B248" s="5"/>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="B249" s="5"/>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="B250" s="5"/>
+    </row>
+    <row r="251" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A251" s="8" t="s">
+        <v>810</v>
+      </c>
+      <c r="B251" s="5"/>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252" s="8"/>
+      <c r="B252" s="5"/>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="B253" s="5"/>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254" s="8" t="s">
+        <v>795</v>
+      </c>
+      <c r="B254" s="5"/>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" s="8"/>
+      <c r="B255" s="5"/>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256" s="9" t="s">
+        <v>655</v>
+      </c>
+      <c r="B256" s="5"/>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257" s="8" t="s">
         <v>794</v>
       </c>
-      <c r="B238" s="5"/>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A239" s="8"/>
-      <c r="B239" s="5"/>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A240" s="9" t="s">
+      <c r="B257" s="5"/>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A258" s="8"/>
+      <c r="B258" s="5"/>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A259" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="B240" s="5"/>
-    </row>
-    <row r="241" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A241" s="8" t="s">
+      <c r="B259" s="5"/>
+    </row>
+    <row r="260" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A260" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="B241" s="5"/>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A242" s="8"/>
-      <c r="B242" s="5"/>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A243" s="9" t="s">
+      <c r="B260" s="5"/>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261" s="8"/>
+      <c r="B261" s="5"/>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262" s="9" t="s">
         <v>680</v>
       </c>
-      <c r="B243" s="5"/>
-    </row>
-    <row r="244" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A244" s="8" t="s">
+      <c r="B262" s="5"/>
+    </row>
+    <row r="263" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A263" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B244" s="5"/>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A245" s="8"/>
-      <c r="B245" s="5"/>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A246" s="8"/>
-      <c r="B246" s="5"/>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A247" s="7" t="s">
-        <v>663</v>
-      </c>
-      <c r="B247" s="5"/>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A248" s="9" t="s">
+      <c r="B263" s="5"/>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264" s="8"/>
+      <c r="B264" s="5"/>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265" s="8"/>
+      <c r="B265" s="5"/>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="B266" s="5"/>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="B248" s="5"/>
-    </row>
-    <row r="249" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A249" s="8" t="s">
-        <v>811</v>
-      </c>
-      <c r="B249" s="5"/>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A250" s="8"/>
-      <c r="B250" s="5"/>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A251" s="9" t="s">
-        <v>654</v>
-      </c>
-      <c r="B251" s="5"/>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A252" s="8" t="s">
-        <v>796</v>
-      </c>
-      <c r="B252" s="5"/>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A253" s="8"/>
-      <c r="B253" s="5"/>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A254" s="9" t="s">
-        <v>655</v>
-      </c>
-      <c r="B254" s="5"/>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A255" s="8" t="s">
-        <v>795</v>
-      </c>
-      <c r="B255" s="5"/>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A256" s="8"/>
-      <c r="B256" s="5"/>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A257" s="9" t="s">
-        <v>656</v>
-      </c>
-      <c r="B257" s="5"/>
-    </row>
-    <row r="258" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A258" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="B258" s="5"/>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A259" s="8"/>
-      <c r="B259" s="5"/>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A260" s="9" t="s">
-        <v>680</v>
-      </c>
-      <c r="B260" s="5"/>
-    </row>
-    <row r="261" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A261" s="8" t="s">
-        <v>695</v>
-      </c>
-      <c r="B261" s="5"/>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A262" s="8"/>
-      <c r="B262" s="5"/>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A263" s="8"/>
-      <c r="B263" s="5"/>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A264" s="7" t="s">
-        <v>664</v>
-      </c>
-      <c r="B264" s="5"/>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A265" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="B265" s="5"/>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A266" s="8" t="s">
+      <c r="B267" s="5"/>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268" s="8" t="s">
         <v>761</v>
-      </c>
-      <c r="B266" s="5"/>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A267" s="8" t="s">
-        <v>791</v>
-      </c>
-      <c r="B267" s="5"/>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A268" s="10" t="s">
-        <v>792</v>
       </c>
       <c r="B268" s="5"/>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="B269" s="5"/>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270" s="10" t="s">
+        <v>791</v>
+      </c>
+      <c r="B270" s="5"/>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271" s="8" t="s">
+        <v>792</v>
+      </c>
+      <c r="B271" s="5"/>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272" s="8" t="s">
         <v>793</v>
       </c>
-      <c r="B269" s="5"/>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A270" s="8" t="s">
-        <v>794</v>
-      </c>
-      <c r="B270" s="5"/>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A271" s="8"/>
-      <c r="B271" s="5"/>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A272" s="9" t="s">
+      <c r="B272" s="5"/>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273" s="8"/>
+      <c r="B273" s="5"/>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="B272" s="5"/>
-    </row>
-    <row r="273" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A273" s="8" t="s">
-        <v>813</v>
-      </c>
-      <c r="B273" s="5"/>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A274" s="8"/>
       <c r="B274" s="5"/>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A275" s="9" t="s">
+    <row r="275" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A275" s="8" t="s">
+        <v>812</v>
+      </c>
+      <c r="B275" s="5"/>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276" s="8"/>
+      <c r="B276" s="5"/>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277" s="9" t="s">
         <v>655</v>
-      </c>
-      <c r="B275" s="5"/>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A276" s="8" t="s">
-        <v>712</v>
-      </c>
-      <c r="B276" s="5"/>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A277" s="8" t="s">
-        <v>814</v>
       </c>
       <c r="B277" s="5"/>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" s="8" t="s">
+        <v>712</v>
+      </c>
+      <c r="B278" s="5"/>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279" s="8" t="s">
+        <v>813</v>
+      </c>
+      <c r="B279" s="5"/>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280" s="8" t="s">
+        <v>814</v>
+      </c>
+      <c r="B280" s="5"/>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281" s="8"/>
+      <c r="B281" s="5"/>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="B282" s="5"/>
+    </row>
+    <row r="283" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A283" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="B283" s="5"/>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284" s="8"/>
+      <c r="B284" s="5"/>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="B285" s="5"/>
+    </row>
+    <row r="286" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A286" s="8" t="s">
+        <v>695</v>
+      </c>
+      <c r="B286" s="5"/>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A287" s="8"/>
+      <c r="B287" s="5"/>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A288" s="8"/>
+      <c r="B288" s="5"/>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A289" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="B289" s="5"/>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A290" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="B290" s="5"/>
+    </row>
+    <row r="291" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A291" s="8" t="s">
         <v>815</v>
       </c>
-      <c r="B278" s="5"/>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A279" s="8"/>
-      <c r="B279" s="5"/>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A280" s="9" t="s">
-        <v>656</v>
-      </c>
-      <c r="B280" s="5"/>
-    </row>
-    <row r="281" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A281" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="B281" s="5"/>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A282" s="8"/>
-      <c r="B282" s="5"/>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A283" s="9" t="s">
-        <v>680</v>
-      </c>
-      <c r="B283" s="5"/>
-    </row>
-    <row r="284" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A284" s="8" t="s">
-        <v>695</v>
-      </c>
-      <c r="B284" s="5"/>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A285" s="8"/>
-      <c r="B285" s="5"/>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A286" s="8"/>
-      <c r="B286" s="5"/>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A287" s="7" t="s">
-        <v>665</v>
-      </c>
-      <c r="B287" s="5"/>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A288" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="B288" s="5"/>
-    </row>
-    <row r="289" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A289" s="8" t="s">
+      <c r="B291" s="5"/>
+    </row>
+    <row r="292" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A292" s="8" t="s">
         <v>816</v>
       </c>
-      <c r="B289" s="5"/>
-    </row>
-    <row r="290" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A290" s="8" t="s">
-        <v>817</v>
-      </c>
-      <c r="B290" s="5"/>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A291" s="8"/>
-      <c r="B291" s="5"/>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A292" s="9" t="s">
+      <c r="B292" s="5"/>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A293" s="8"/>
+      <c r="B293" s="5"/>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A294" s="9" t="s">
         <v>654</v>
-      </c>
-      <c r="B292" s="5"/>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A293" s="8" t="s">
-        <v>802</v>
-      </c>
-      <c r="B293" s="5"/>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A294" s="8" t="s">
-        <v>803</v>
       </c>
       <c r="B294" s="5"/>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" s="8" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="B295" s="5"/>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" s="8" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="B296" s="5"/>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" s="8" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B297" s="5"/>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A298" s="8"/>
+      <c r="A298" s="8" t="s">
+        <v>804</v>
+      </c>
       <c r="B298" s="5"/>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A299" s="9" t="s">
+      <c r="A299" s="8" t="s">
+        <v>805</v>
+      </c>
+      <c r="B299" s="5"/>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A300" s="8"/>
+      <c r="B300" s="5"/>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A301" s="9" t="s">
         <v>655</v>
-      </c>
-      <c r="B299" s="5"/>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A300" s="8" t="s">
-        <v>712</v>
-      </c>
-      <c r="B300" s="5"/>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A301" s="8" t="s">
-        <v>763</v>
       </c>
       <c r="B301" s="5"/>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" s="8" t="s">
-        <v>818</v>
+        <v>712</v>
       </c>
       <c r="B302" s="5"/>
     </row>
@@ -51369,991 +51369,1006 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" s="8" t="s">
+        <v>817</v>
+      </c>
+      <c r="B304" s="5"/>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A305" s="8" t="s">
+        <v>763</v>
+      </c>
+      <c r="B305" s="5"/>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A306" s="8" t="s">
         <v>712</v>
       </c>
-      <c r="B304" s="5"/>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A305" s="8"/>
-      <c r="B305" s="5"/>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A306" s="9" t="s">
+      <c r="B306" s="5"/>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A307" s="8"/>
+      <c r="B307" s="5"/>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A308" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="B306" s="5"/>
-    </row>
-    <row r="307" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A307" s="8" t="s">
+      <c r="B308" s="5"/>
+    </row>
+    <row r="309" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A309" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="B307" s="5"/>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A308" s="8"/>
-      <c r="B308" s="5"/>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A309" s="9" t="s">
+      <c r="B309" s="5"/>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A310" s="8"/>
+      <c r="B310" s="5"/>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A311" s="9" t="s">
         <v>680</v>
       </c>
-      <c r="B309" s="5"/>
-    </row>
-    <row r="310" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A310" s="8" t="s">
+      <c r="B311" s="5"/>
+    </row>
+    <row r="312" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A312" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B310" s="5"/>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A311" s="8"/>
-      <c r="B311" s="5"/>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A312" s="8"/>
       <c r="B312" s="5"/>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A313" s="7" t="s">
+      <c r="A313" s="8"/>
+      <c r="B313" s="5"/>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A314" s="8"/>
+      <c r="B314" s="5"/>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A315" s="7" t="s">
         <v>666</v>
       </c>
-      <c r="B313" s="5"/>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A314" s="9" t="s">
+      <c r="B315" s="5"/>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A316" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="B314" s="5"/>
-    </row>
-    <row r="315" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A315" s="8" t="s">
-        <v>811</v>
-      </c>
-      <c r="B315" s="5"/>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A316" s="8"/>
       <c r="B316" s="5"/>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A317" s="9" t="s">
+    <row r="317" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A317" s="8" t="s">
+        <v>810</v>
+      </c>
+      <c r="B317" s="5"/>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A318" s="8"/>
+      <c r="B318" s="5"/>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A319" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="B317" s="5"/>
-    </row>
-    <row r="318" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A318" s="8" t="s">
+      <c r="B319" s="5"/>
+    </row>
+    <row r="320" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A320" s="8" t="s">
+        <v>818</v>
+      </c>
+      <c r="B320" s="5"/>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A321" s="8"/>
+      <c r="B321" s="5"/>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A322" s="9" t="s">
+        <v>655</v>
+      </c>
+      <c r="B322" s="5"/>
+    </row>
+    <row r="323" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A323" s="8" t="s">
         <v>819</v>
       </c>
-      <c r="B318" s="5"/>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A319" s="8"/>
-      <c r="B319" s="5"/>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A320" s="9" t="s">
-        <v>655</v>
-      </c>
-      <c r="B320" s="5"/>
-    </row>
-    <row r="321" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A321" s="8" t="s">
+      <c r="B323" s="5"/>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A324" s="8"/>
+      <c r="B324" s="5"/>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A325" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="B325" s="5"/>
+    </row>
+    <row r="326" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A326" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="B326" s="5"/>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A327" s="8"/>
+      <c r="B327" s="5"/>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A328" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="B328" s="5"/>
+    </row>
+    <row r="329" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A329" s="8" t="s">
+        <v>695</v>
+      </c>
+      <c r="B329" s="5"/>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A330" s="8"/>
+      <c r="B330" s="5"/>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A331" s="8"/>
+      <c r="B331" s="5"/>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A332" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="B332" s="5"/>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A333" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="B333" s="5"/>
+    </row>
+    <row r="334" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A334" s="8" t="s">
         <v>820</v>
       </c>
-      <c r="B321" s="5"/>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A322" s="8"/>
-      <c r="B322" s="5"/>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A323" s="9" t="s">
-        <v>656</v>
-      </c>
-      <c r="B323" s="5"/>
-    </row>
-    <row r="324" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A324" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="B324" s="5"/>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A325" s="8"/>
-      <c r="B325" s="5"/>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A326" s="9" t="s">
-        <v>680</v>
-      </c>
-      <c r="B326" s="5"/>
-    </row>
-    <row r="327" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A327" s="8" t="s">
-        <v>695</v>
-      </c>
-      <c r="B327" s="5"/>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A328" s="8"/>
-      <c r="B328" s="5"/>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A329" s="8"/>
-      <c r="B329" s="5"/>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A330" s="7" t="s">
-        <v>667</v>
-      </c>
-      <c r="B330" s="5"/>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A331" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="B331" s="5"/>
-    </row>
-    <row r="332" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A332" s="8" t="s">
-        <v>821</v>
-      </c>
-      <c r="B332" s="5"/>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A333" s="8"/>
-      <c r="B333" s="5"/>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A334" s="9" t="s">
+      <c r="B334" s="5"/>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A335" s="8"/>
+      <c r="B335" s="5"/>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A336" s="9" t="s">
         <v>654</v>
-      </c>
-      <c r="B334" s="5"/>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A335" s="8" t="s">
-        <v>809</v>
-      </c>
-      <c r="B335" s="5"/>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A336" s="8" t="s">
-        <v>810</v>
       </c>
       <c r="B336" s="5"/>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" s="8" t="s">
-        <v>802</v>
+        <v>808</v>
       </c>
       <c r="B337" s="5"/>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" s="8" t="s">
-        <v>803</v>
+        <v>809</v>
       </c>
       <c r="B338" s="5"/>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" s="8" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="B339" s="5"/>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" s="8" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="B340" s="5"/>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" s="8" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B341" s="5"/>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A342" s="8"/>
+      <c r="A342" s="8" t="s">
+        <v>804</v>
+      </c>
       <c r="B342" s="5"/>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A343" s="9" t="s">
+      <c r="A343" s="8" t="s">
+        <v>805</v>
+      </c>
+      <c r="B343" s="5"/>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A344" s="8"/>
+      <c r="B344" s="5"/>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A345" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="B343" s="5"/>
-    </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A344" s="8" t="s">
-        <v>795</v>
-      </c>
-      <c r="B344" s="5"/>
-    </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A345" s="8"/>
       <c r="B345" s="5"/>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A346" s="9" t="s">
+      <c r="A346" s="8" t="s">
+        <v>794</v>
+      </c>
+      <c r="B346" s="5"/>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A347" s="8"/>
+      <c r="B347" s="5"/>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A348" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="B346" s="5"/>
-    </row>
-    <row r="347" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A347" s="8" t="s">
+      <c r="B348" s="5"/>
+    </row>
+    <row r="349" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A349" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="B347" s="5"/>
-    </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A348" s="8"/>
-      <c r="B348" s="5"/>
-    </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A349" s="9" t="s">
+      <c r="B349" s="5"/>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A350" s="8"/>
+      <c r="B350" s="5"/>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A351" s="9" t="s">
         <v>680</v>
       </c>
-      <c r="B349" s="5"/>
-    </row>
-    <row r="350" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A350" s="8" t="s">
+      <c r="B351" s="5"/>
+    </row>
+    <row r="352" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A352" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B350" s="5"/>
-    </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A351" s="8"/>
-      <c r="B351" s="5"/>
-    </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A352" s="8"/>
-      <c r="B352" s="8" t="s">
+      <c r="B352" s="5"/>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A353" s="8"/>
+      <c r="B353" s="5"/>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A354" s="8"/>
+      <c r="B354" s="5"/>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A355" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="B355" s="8" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A353" s="7" t="s">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A356" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="B356" s="7" t="s">
         <v>669</v>
       </c>
-      <c r="B353" s="7" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A354" s="9" t="s">
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A357" s="8" t="s">
+        <v>821</v>
+      </c>
+      <c r="B357" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="B354" s="9" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A355" s="8" t="s">
-        <v>822</v>
-      </c>
-      <c r="B355" s="8" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A356" s="8"/>
-      <c r="B356" s="8"/>
-    </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A357" s="9" t="s">
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A358" s="8"/>
+      <c r="B358" s="8" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A359" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="B357" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A358" s="8" t="s">
-        <v>823</v>
-      </c>
-      <c r="B358" s="8" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A359" s="8" t="s">
-        <v>824</v>
-      </c>
-      <c r="B359" s="8" t="s">
-        <v>824</v>
-      </c>
+      <c r="B359" s="8"/>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" s="8" t="s">
-        <v>825</v>
-      </c>
-      <c r="B360" s="8" t="s">
-        <v>825</v>
+        <v>822</v>
+      </c>
+      <c r="B360" s="9" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A361" s="8"/>
-      <c r="B361" s="8"/>
+      <c r="A361" s="8" t="s">
+        <v>823</v>
+      </c>
+      <c r="B361" s="8" t="s">
+        <v>822</v>
+      </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A362" s="9" t="s">
+      <c r="A362" s="8" t="s">
+        <v>824</v>
+      </c>
+      <c r="B362" s="8" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A363" s="8"/>
+      <c r="B363" s="8" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A364" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="B362" s="9" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A363" s="8" t="s">
-        <v>761</v>
-      </c>
-      <c r="B363" s="8" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A364" s="10" t="s">
-        <v>791</v>
-      </c>
-      <c r="B364" s="10" t="s">
-        <v>791</v>
-      </c>
+      <c r="B364" s="8"/>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" s="8" t="s">
-        <v>792</v>
-      </c>
-      <c r="B365" s="8" t="s">
-        <v>792</v>
+        <v>761</v>
+      </c>
+      <c r="B365" s="9" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" s="10" t="s">
+        <v>790</v>
+      </c>
+      <c r="B366" s="8" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A367" s="8" t="s">
+        <v>791</v>
+      </c>
+      <c r="B367" s="10" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A368" s="10" t="s">
+        <v>792</v>
+      </c>
+      <c r="B368" s="8" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A369" s="10" t="s">
         <v>793</v>
       </c>
-      <c r="B366" s="10" t="s">
+      <c r="B369" s="10" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A370" s="8"/>
+      <c r="B370" s="10" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A367" s="10" t="s">
-        <v>794</v>
-      </c>
-      <c r="B367" s="10" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A368" s="8"/>
-      <c r="B368" s="8"/>
-    </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A369" s="9" t="s">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A371" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="B369" s="9" t="s">
+      <c r="B371" s="8"/>
+    </row>
+    <row r="372" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A372" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="B372" s="9" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="370" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A370" s="8" t="s">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A373" s="8"/>
+      <c r="B373" s="8" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A374" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="B374" s="8"/>
+    </row>
+    <row r="375" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A375" s="8" t="s">
+        <v>695</v>
+      </c>
+      <c r="B375" s="8"/>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A376" s="8"/>
+      <c r="B376" s="8"/>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A377" s="8"/>
+      <c r="B377" s="8"/>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A378" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="B378" s="8"/>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A379" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="B379" s="7" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A380" s="8" t="s">
+        <v>825</v>
+      </c>
+      <c r="B380" s="9" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A381" s="8" t="s">
+        <v>712</v>
+      </c>
+      <c r="B381" s="8" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A382" s="8"/>
+      <c r="B382" s="8" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A383" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="B383" s="8"/>
+    </row>
+    <row r="384" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A384" s="8" t="s">
+        <v>826</v>
+      </c>
+      <c r="B384" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A385" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="B385" s="8" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A386" s="8" t="s">
+        <v>827</v>
+      </c>
+      <c r="B386" s="8" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A387" s="8"/>
+      <c r="B387" s="8" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A388" s="9" t="s">
+        <v>655</v>
+      </c>
+      <c r="B388" s="8"/>
+    </row>
+    <row r="389" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A389" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="B370" s="8" t="s">
+      <c r="B389" s="9" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A390" s="8"/>
+      <c r="B390" s="10" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A371" s="8"/>
-      <c r="B371" s="8"/>
-    </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A372" s="9" t="s">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A391" s="9" t="s">
         <v>680</v>
       </c>
-      <c r="B372" s="8"/>
-    </row>
-    <row r="373" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A373" s="8" t="s">
+      <c r="B391" s="8"/>
+    </row>
+    <row r="392" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A392" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B373" s="8"/>
-    </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A374" s="8"/>
-      <c r="B374" s="8"/>
-    </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A375" s="8"/>
-      <c r="B375" s="8"/>
-    </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A376" s="7" t="s">
-        <v>670</v>
-      </c>
-      <c r="B376" s="7" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A377" s="9" t="s">
+      <c r="B392" s="8"/>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A393" s="8"/>
+      <c r="B393" s="8"/>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A394" s="8"/>
+      <c r="B394" s="8"/>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A395" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="B395" s="8"/>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A396" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="B377" s="9" t="s">
+      <c r="B396" s="7" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A397" s="8" t="s">
+        <v>795</v>
+      </c>
+      <c r="B397" s="9" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A378" s="8" t="s">
-        <v>826</v>
-      </c>
-      <c r="B378" s="8" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A379" s="8" t="s">
-        <v>712</v>
-      </c>
-      <c r="B379" s="8" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A380" s="8"/>
-      <c r="B380" s="8"/>
-    </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A381" s="9" t="s">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A398" s="8"/>
+      <c r="B398" s="8" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A399" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="B381" s="9" t="s">
+      <c r="B399" s="8"/>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A400" s="8" t="s">
+        <v>761</v>
+      </c>
+      <c r="B400" s="9" t="s">
         <v>654</v>
-      </c>
-    </row>
-    <row r="382" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A382" s="8" t="s">
-        <v>827</v>
-      </c>
-      <c r="B382" s="8" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A383" s="8" t="s">
-        <v>719</v>
-      </c>
-      <c r="B383" s="8" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A384" s="8" t="s">
-        <v>828</v>
-      </c>
-      <c r="B384" s="8" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A385" s="8"/>
-      <c r="B385" s="8"/>
-    </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A386" s="9" t="s">
-        <v>655</v>
-      </c>
-      <c r="B386" s="9" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="387" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A387" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="B387" s="10" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A388" s="8"/>
-      <c r="B388" s="8"/>
-    </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A389" s="9" t="s">
-        <v>680</v>
-      </c>
-      <c r="B389" s="8"/>
-    </row>
-    <row r="390" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A390" s="8" t="s">
-        <v>695</v>
-      </c>
-      <c r="B390" s="8"/>
-    </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A391" s="8"/>
-      <c r="B391" s="8"/>
-    </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A392" s="8"/>
-      <c r="B392" s="8"/>
-    </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A393" s="7" t="s">
-        <v>671</v>
-      </c>
-      <c r="B393" s="7" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A394" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="B394" s="9" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A395" s="8" t="s">
-        <v>796</v>
-      </c>
-      <c r="B395" s="8" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A396" s="8"/>
-      <c r="B396" s="8"/>
-    </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A397" s="9" t="s">
-        <v>654</v>
-      </c>
-      <c r="B397" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A398" s="8" t="s">
-        <v>761</v>
-      </c>
-      <c r="B398" s="8" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A399" s="10" t="s">
-        <v>791</v>
-      </c>
-      <c r="B399" s="10" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A400" s="10" t="s">
-        <v>792</v>
-      </c>
-      <c r="B400" s="10" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" s="10" t="s">
-        <v>793</v>
-      </c>
-      <c r="B401" s="10" t="s">
-        <v>793</v>
+        <v>790</v>
+      </c>
+      <c r="B401" s="8" t="s">
+        <v>761</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" s="10" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="B402" s="10" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A403" s="8"/>
-      <c r="B403" s="8"/>
+      <c r="A403" s="10" t="s">
+        <v>792</v>
+      </c>
+      <c r="B403" s="10" t="s">
+        <v>791</v>
+      </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A404" s="9" t="s">
+      <c r="A404" s="10" t="s">
+        <v>793</v>
+      </c>
+      <c r="B404" s="10" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A405" s="8"/>
+      <c r="B405" s="10" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A406" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="B404" s="9" t="s">
+      <c r="B406" s="8"/>
+    </row>
+    <row r="407" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A407" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="B407" s="9" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="405" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A405" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="B405" s="10" t="s">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A408" s="8"/>
+      <c r="B408" s="10" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A406" s="8"/>
-      <c r="B406" s="8"/>
-    </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A407" s="9" t="s">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A409" s="9" t="s">
         <v>680</v>
       </c>
-      <c r="B407" s="8"/>
-    </row>
-    <row r="408" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A408" s="8" t="s">
+      <c r="B409" s="8"/>
+    </row>
+    <row r="410" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A410" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B408" s="8"/>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A409" s="8"/>
-      <c r="B409" s="8"/>
-    </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A410" s="8"/>
       <c r="B410" s="8"/>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A411" s="7" t="s">
+      <c r="A411" s="8"/>
+      <c r="B411" s="8"/>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A412" s="8"/>
+      <c r="B412" s="8"/>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A413" s="7" t="s">
         <v>672</v>
       </c>
-      <c r="B411" s="7" t="s">
+      <c r="B413" s="8"/>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A414" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="B414" s="7" t="s">
         <v>672</v>
-      </c>
-    </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A412" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="B412" s="9" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A413" s="8" t="s">
-        <v>822</v>
-      </c>
-      <c r="B413" s="8" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A414" s="8" t="s">
-        <v>808</v>
-      </c>
-      <c r="B414" s="8" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415" s="8" t="s">
-        <v>829</v>
-      </c>
-      <c r="B415" s="8" t="s">
-        <v>829</v>
+        <v>821</v>
+      </c>
+      <c r="B415" s="9" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A416" s="8"/>
-      <c r="B416" s="8"/>
+      <c r="A416" s="8" t="s">
+        <v>807</v>
+      </c>
+      <c r="B416" s="8" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A417" s="9" t="s">
+      <c r="A417" s="8" t="s">
+        <v>828</v>
+      </c>
+      <c r="B417" s="8" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A418" s="8"/>
+      <c r="B418" s="8" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A419" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="B417" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A418" s="8" t="s">
-        <v>712</v>
-      </c>
-      <c r="B418" s="8" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A419" s="8" t="s">
-        <v>814</v>
-      </c>
-      <c r="B419" s="8" t="s">
-        <v>814</v>
-      </c>
+      <c r="B419" s="8"/>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" s="8" t="s">
+        <v>712</v>
+      </c>
+      <c r="B420" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A421" s="8" t="s">
+        <v>813</v>
+      </c>
+      <c r="B421" s="8" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A422" s="8" t="s">
         <v>763</v>
       </c>
-      <c r="B420" s="8" t="s">
+      <c r="B422" s="8" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A423" s="8"/>
+      <c r="B423" s="8" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A421" s="8"/>
-      <c r="B421" s="8"/>
-    </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A422" s="9" t="s">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A424" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="B422" s="9" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A423" s="8" t="s">
-        <v>830</v>
-      </c>
-      <c r="B423" s="8" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A424" s="8" t="s">
-        <v>824</v>
-      </c>
-      <c r="B424" s="8" t="s">
-        <v>824</v>
-      </c>
+      <c r="B424" s="8"/>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A425" s="8" t="s">
+        <v>829</v>
+      </c>
+      <c r="B425" s="9" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A426" s="8" t="s">
+        <v>823</v>
+      </c>
+      <c r="B426" s="8" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A427" s="8" t="s">
         <v>712</v>
       </c>
-      <c r="B425" s="8" t="s">
+      <c r="B427" s="8" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A428" s="8"/>
+      <c r="B428" s="8" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A426" s="8"/>
-      <c r="B426" s="8"/>
-    </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A427" s="9" t="s">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A429" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="B427" s="9" t="s">
+      <c r="B429" s="8"/>
+    </row>
+    <row r="430" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A430" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="B430" s="9" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="428" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A428" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="B428" s="10" t="s">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A431" s="8"/>
+      <c r="B431" s="10" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A429" s="8"/>
-      <c r="B429" s="8"/>
-    </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A430" s="9" t="s">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A432" s="9" t="s">
         <v>680</v>
       </c>
-      <c r="B430" s="8"/>
-    </row>
-    <row r="431" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A431" s="8" t="s">
+      <c r="B432" s="8"/>
+    </row>
+    <row r="433" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A433" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B431" s="8"/>
-    </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A432" s="8"/>
-      <c r="B432" s="8"/>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A433" s="8"/>
       <c r="B433" s="8"/>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A434" s="7" t="s">
+      <c r="A434" s="8"/>
+      <c r="B434" s="8"/>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A435" s="8"/>
+      <c r="B435" s="8"/>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A436" s="7" t="s">
         <v>673</v>
       </c>
-      <c r="B434" s="7" t="s">
+      <c r="B436" s="8"/>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A437" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="B437" s="7" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A435" s="9" t="s">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A438" s="8" t="s">
+        <v>830</v>
+      </c>
+      <c r="B438" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="B435" s="9" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A436" s="8" t="s">
-        <v>831</v>
-      </c>
-      <c r="B436" s="8" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A437" s="8"/>
-      <c r="B437" s="8"/>
-    </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A438" s="9" t="s">
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A439" s="8"/>
+      <c r="B439" s="8" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A440" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="B438" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A439" s="8" t="s">
-        <v>712</v>
-      </c>
-      <c r="B439" s="8" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A440" s="8" t="s">
-        <v>814</v>
-      </c>
-      <c r="B440" s="8" t="s">
-        <v>814</v>
-      </c>
+      <c r="B440" s="8"/>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" s="8" t="s">
+        <v>712</v>
+      </c>
+      <c r="B441" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A442" s="8" t="s">
+        <v>813</v>
+      </c>
+      <c r="B442" s="8" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A443" s="8" t="s">
         <v>763</v>
       </c>
-      <c r="B441" s="8" t="s">
+      <c r="B443" s="8" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A444" s="8"/>
+      <c r="B444" s="8" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A442" s="8"/>
-      <c r="B442" s="8"/>
-    </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A443" s="9" t="s">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A445" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="B443" s="9" t="s">
+      <c r="B445" s="8"/>
+    </row>
+    <row r="446" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A446" s="8" t="s">
+        <v>831</v>
+      </c>
+      <c r="B446" s="9" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="444" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A444" s="8" t="s">
+    <row r="447" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A447" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="B447" s="8" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A448" s="8" t="s">
+        <v>827</v>
+      </c>
+      <c r="B448" s="8" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A449" s="8"/>
+      <c r="B449" s="8" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A450" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="B450" s="8"/>
+    </row>
+    <row r="451" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A451" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="B451" s="9" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A452" s="8"/>
+      <c r="B452" s="10" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A453" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="B453" s="8"/>
+    </row>
+    <row r="454" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A454" s="8" t="s">
+        <v>695</v>
+      </c>
+      <c r="B454" s="5"/>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A455" s="8"/>
+      <c r="B455" s="5"/>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A456" s="8"/>
+      <c r="B456" s="5"/>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A457" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="B457" s="5"/>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A458" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="B458" s="5"/>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A459" s="8" t="s">
         <v>832</v>
       </c>
-      <c r="B444" s="8" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A445" s="8" t="s">
-        <v>719</v>
-      </c>
-      <c r="B445" s="8" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A446" s="8" t="s">
-        <v>828</v>
-      </c>
-      <c r="B446" s="8" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A447" s="8"/>
-      <c r="B447" s="8"/>
-    </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A448" s="9" t="s">
-        <v>656</v>
-      </c>
-      <c r="B448" s="9" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="449" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A449" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="B449" s="10" t="s">
+      <c r="B459" s="5"/>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A460" s="8" t="s">
+        <v>833</v>
+      </c>
+      <c r="B460" s="5"/>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A461" s="8"/>
+      <c r="B461" s="5"/>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A462" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="B462" s="5"/>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A463" s="8" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A450" s="8"/>
-      <c r="B450" s="8"/>
-    </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A451" s="9" t="s">
-        <v>680</v>
-      </c>
-      <c r="B451" s="5"/>
-    </row>
-    <row r="452" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A452" s="8" t="s">
-        <v>695</v>
-      </c>
-      <c r="B452" s="5"/>
-    </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A453" s="8"/>
-      <c r="B453" s="5"/>
-    </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A454" s="8"/>
-      <c r="B454" s="5"/>
-    </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A455" s="7" t="s">
-        <v>674</v>
-      </c>
-      <c r="B455" s="5"/>
-    </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A456" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="B456" s="5"/>
-    </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A457" s="8" t="s">
-        <v>833</v>
-      </c>
-      <c r="B457" s="5"/>
-    </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A458" s="8" t="s">
-        <v>834</v>
-      </c>
-      <c r="B458" s="5"/>
-    </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A459" s="8"/>
-      <c r="B459" s="5"/>
-    </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A460" s="9" t="s">
-        <v>654</v>
-      </c>
-      <c r="B460" s="5"/>
-    </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A461" s="8" t="s">
-        <v>668</v>
-      </c>
-      <c r="B461" s="5"/>
+      <c r="B463" s="5"/>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B464" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -52364,7 +52379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A1B52C-F7FD-4E7F-BB69-7226FA734E9B}">
   <dimension ref="A1:B417"/>
   <sheetViews>
-    <sheetView topLeftCell="A391" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
       <selection activeCell="A228" sqref="A228"/>
     </sheetView>
   </sheetViews>
@@ -52657,7 +52672,7 @@
     </row>
     <row r="54" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B54" s="5"/>
     </row>
@@ -52673,13 +52688,13 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B57" s="5"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B58" s="5"/>
     </row>
@@ -52711,13 +52726,13 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B65" s="5"/>
     </row>
@@ -52759,7 +52774,7 @@
     </row>
     <row r="73" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B73" s="5"/>
     </row>
@@ -52775,13 +52790,13 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B76" s="5"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B77" s="5"/>
     </row>
@@ -52813,13 +52828,13 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B83" s="5"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B84" s="5"/>
     </row>
@@ -52861,7 +52876,7 @@
     </row>
     <row r="92" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B92" s="5"/>
     </row>
@@ -52877,13 +52892,13 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B95" s="5"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B96" s="5"/>
     </row>
@@ -52899,7 +52914,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B99" s="5"/>
     </row>
@@ -52915,13 +52930,13 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B102" s="5"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B103" s="5"/>
     </row>
@@ -52963,7 +52978,7 @@
     </row>
     <row r="111" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B111" s="5"/>
     </row>
@@ -52979,7 +52994,7 @@
     </row>
     <row r="114" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B114" s="5"/>
     </row>
@@ -52989,25 +53004,25 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B116" s="5"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B117" s="5"/>
     </row>
     <row r="118" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="8" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B118" s="5"/>
     </row>
     <row r="119" spans="1:2" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A119" s="24" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B119" s="5"/>
     </row>
@@ -53033,19 +53048,19 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B124" s="5"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="8" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B125" s="5"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B126" s="5"/>
     </row>
@@ -53083,7 +53098,7 @@
     </row>
     <row r="133" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B133" s="5"/>
     </row>
@@ -53093,19 +53108,19 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B135" s="5"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B136" s="5"/>
     </row>
     <row r="137" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A137" s="8" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B137" s="5"/>
     </row>
@@ -53137,13 +53152,13 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="8" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B143" s="5"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="8" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B144" s="5"/>
     </row>
@@ -53159,7 +53174,7 @@
     </row>
     <row r="147" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A147" s="8" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B147" s="5"/>
     </row>
@@ -53175,7 +53190,7 @@
     </row>
     <row r="150" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A150" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B150" s="5"/>
     </row>
@@ -53185,19 +53200,19 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B152" s="5"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B153" s="5"/>
     </row>
     <row r="154" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A154" s="8" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B154" s="5"/>
     </row>
@@ -53223,7 +53238,7 @@
     </row>
     <row r="159" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A159" s="8" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B159" s="5"/>
     </row>
@@ -53239,7 +53254,7 @@
     </row>
     <row r="162" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A162" s="8" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B162" s="5"/>
     </row>
@@ -53249,19 +53264,19 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B164" s="5"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B165" s="5"/>
     </row>
     <row r="166" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A166" s="8" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B166" s="5"/>
     </row>
@@ -53293,13 +53308,13 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="8" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B172" s="5"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="8" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B173" s="5"/>
     </row>
@@ -53321,7 +53336,7 @@
     </row>
     <row r="177" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A177" s="8" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B177" s="5"/>
     </row>
@@ -53337,7 +53352,7 @@
     </row>
     <row r="180" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A180" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B180" s="5"/>
     </row>
@@ -53347,19 +53362,19 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B182" s="5"/>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B183" s="5"/>
     </row>
     <row r="184" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A184" s="8" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B184" s="5"/>
     </row>
@@ -53391,7 +53406,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="8" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B190" s="5"/>
     </row>
@@ -53413,7 +53428,7 @@
     </row>
     <row r="194" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A194" s="8" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B194" s="5"/>
     </row>
@@ -53429,7 +53444,7 @@
     </row>
     <row r="197" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A197" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B197" s="5"/>
     </row>
@@ -53439,19 +53454,19 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B199" s="5"/>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B200" s="5"/>
     </row>
     <row r="201" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A201" s="8" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B201" s="5"/>
     </row>
@@ -53477,7 +53492,7 @@
     </row>
     <row r="206" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A206" s="8" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B206" s="5"/>
     </row>
@@ -53499,7 +53514,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="8" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B210" s="5"/>
     </row>
@@ -53515,19 +53530,19 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B213" s="5"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B214" s="5"/>
     </row>
     <row r="215" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A215" s="8" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B215" s="5"/>
     </row>
@@ -53559,19 +53574,19 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="8" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B221" s="5"/>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="8" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B222" s="5"/>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="8" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B223" s="5"/>
     </row>
@@ -53599,19 +53614,19 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="8" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B228" s="5"/>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="8" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B229" s="5"/>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="8" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B230" s="5"/>
     </row>
@@ -53633,7 +53648,7 @@
     </row>
     <row r="234" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A234" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B234" s="5"/>
     </row>
@@ -53643,19 +53658,19 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B236" s="5"/>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B237" s="5"/>
     </row>
     <row r="238" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A238" s="8" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B238" s="5"/>
     </row>
@@ -53687,7 +53702,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="8" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B244" s="5"/>
     </row>
@@ -53715,13 +53730,13 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" s="8" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B249" s="5"/>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="8" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B250" s="5"/>
     </row>
@@ -53743,7 +53758,7 @@
     </row>
     <row r="254" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A254" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B254" s="5"/>
     </row>
@@ -53753,19 +53768,19 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B256" s="5"/>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B257" s="5"/>
     </row>
     <row r="258" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A258" s="8" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B258" s="5"/>
     </row>
@@ -53791,7 +53806,7 @@
     </row>
     <row r="263" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A263" s="8" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B263" s="5"/>
     </row>
@@ -53813,19 +53828,19 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="8" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B267" s="5"/>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" s="8" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B268" s="5"/>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="8" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B269" s="5"/>
     </row>
@@ -53841,19 +53856,19 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B272" s="5"/>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B273" s="5"/>
     </row>
     <row r="274" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A274" s="8" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B274" s="5"/>
     </row>
@@ -53885,19 +53900,19 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" s="8" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B280" s="5"/>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" s="8" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B281" s="5"/>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" s="8" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B282" s="5"/>
     </row>
@@ -53925,7 +53940,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" s="8" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B287" s="5"/>
     </row>
@@ -53947,7 +53962,7 @@
     </row>
     <row r="291" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A291" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B291" s="5"/>
     </row>
@@ -53957,19 +53972,19 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B293" s="5"/>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B294" s="5"/>
     </row>
     <row r="295" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A295" s="8" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B295" s="5"/>
     </row>
@@ -54001,7 +54016,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="8" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B301" s="5"/>
     </row>
@@ -54029,7 +54044,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" s="8" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B306" s="5"/>
     </row>
@@ -54051,7 +54066,7 @@
     </row>
     <row r="310" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A310" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B310" s="5"/>
     </row>
@@ -54061,19 +54076,19 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B312" s="5"/>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B313" s="5"/>
     </row>
     <row r="314" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A314" s="8" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B314" s="5"/>
     </row>
@@ -54105,10 +54120,10 @@
     </row>
     <row r="319" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A319" s="8" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B319" s="8" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
@@ -54125,10 +54140,10 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" s="8" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B322" s="8" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
@@ -54145,7 +54160,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B325" s="9" t="s">
         <v>655</v>
@@ -54153,7 +54168,7 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B326" s="10" t="s">
         <v>668</v>
@@ -54161,7 +54176,7 @@
     </row>
     <row r="327" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A327" s="8" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B327" s="8"/>
     </row>
@@ -54199,26 +54214,26 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" s="8" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B333" s="8" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" s="8" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B334" s="8" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" s="8" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B335" s="8" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
@@ -54243,26 +54258,26 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" s="8" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B339" s="8" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" s="8" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B340" s="8" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" s="8" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B341" s="8" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
@@ -54279,7 +54294,7 @@
     </row>
     <row r="344" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A344" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B344" s="10" t="s">
         <v>668</v>
@@ -54291,19 +54306,19 @@
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B346" s="8"/>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B347" s="10"/>
     </row>
     <row r="348" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A348" s="8" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B348" s="8"/>
     </row>
@@ -54333,10 +54348,10 @@
     </row>
     <row r="353" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A353" s="8" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B353" s="8" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
@@ -54353,10 +54368,10 @@
     </row>
     <row r="356" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A356" s="8" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B356" s="8" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.2">
@@ -54373,7 +54388,7 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B359" s="9" t="s">
         <v>655</v>
@@ -54381,7 +54396,7 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B360" s="10" t="s">
         <v>668</v>
@@ -54389,7 +54404,7 @@
     </row>
     <row r="361" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A361" s="8" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B361" s="8"/>
     </row>
@@ -54427,10 +54442,10 @@
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" s="8" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B367" s="8" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.2">
@@ -54455,10 +54470,10 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" s="8" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B371" s="8" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.2">
@@ -54475,7 +54490,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B374" s="9" t="s">
         <v>655</v>
@@ -54483,7 +54498,7 @@
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B375" s="10" t="s">
         <v>668</v>
@@ -54491,7 +54506,7 @@
     </row>
     <row r="376" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A376" s="8" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B376" s="8"/>
     </row>
@@ -54529,18 +54544,18 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" s="8" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B382" s="8" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" s="8" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B383" s="8" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.2">
@@ -54557,10 +54572,10 @@
     </row>
     <row r="386" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A386" s="8" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.2">
@@ -54585,7 +54600,7 @@
     </row>
     <row r="390" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A390" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B390" s="10" t="s">
         <v>668</v>
@@ -54597,19 +54612,19 @@
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B392" s="5"/>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" s="10" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B393" s="5"/>
     </row>
     <row r="394" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A394" s="8" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B394" s="5"/>
     </row>
@@ -54629,13 +54644,13 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" s="9" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B398" s="5"/>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399" s="8" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B399" s="5"/>
     </row>
@@ -54645,13 +54660,13 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" s="9" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B401" s="5"/>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" s="8" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B402" s="5"/>
     </row>
@@ -54661,13 +54676,13 @@
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404" s="9" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B404" s="5"/>
     </row>
     <row r="405" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A405" s="8" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B405" s="5"/>
     </row>
@@ -54677,13 +54692,13 @@
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407" s="9" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B407" s="5"/>
     </row>
     <row r="408" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A408" s="8" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B408" s="5"/>
     </row>
@@ -54693,13 +54708,13 @@
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A410" s="9" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B410" s="5"/>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A411" s="8" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B411" s="5"/>
     </row>
@@ -54709,13 +54724,13 @@
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A413" s="9" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B413" s="5"/>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A414" s="8" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B414" s="5"/>
     </row>
@@ -54725,7 +54740,7 @@
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A416" s="9" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B416" s="5"/>
     </row>

</xml_diff>